<commit_message>
first commit of the summer. Created oh_house_sales_df.dta
</commit_message>
<xml_diff>
--- a/ohio_employment/ohio_employment_project.xlsx
+++ b/ohio_employment/ohio_employment_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rawatsa\OneDrive - University of Cincinnati\StataProjects\ohio_employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{554608AD-74A0-4881-A128-F3CC3303FF3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{719E8C9B-622D-48BA-97B0-01BD11BD56E8}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{554608AD-74A0-4881-A128-F3CC3303FF3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1C5BD18E-FEBA-4F5F-94B6-530D155A2874}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="2" xr2:uid="{806BFF36-45C0-47FA-AF20-9489653F8F2D}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="data_dictionary" sheetId="1" r:id="rId1"/>
     <sheet name="naics_codes" sheetId="3" r:id="rId2"/>
     <sheet name="notes" sheetId="2" r:id="rId3"/>
+    <sheet name="files" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="113">
   <si>
     <t>Data Dictionary</t>
   </si>
@@ -245,7 +246,127 @@
     <t>1. Master datafiles contain observations with "State" variable that is not "Ohio" but has data from other states. Should I keep them or remove?</t>
   </si>
   <si>
-    <t>2. Created a new master df called "". Contains all data from 2006 to 2021Q2. NAICS variable from 2019 is still missing.</t>
+    <t>2. Created master datasets called "masterfile_2006q1_2021q2.sas7bdat" and "masterfile_2006q1_2019q4.sas7bdat". Covers all data from 2006 to 2021Q2. NAICS variable from 2019 is still missing.</t>
+  </si>
+  <si>
+    <t>1. Tried adding NAICS code to year 2019 using 2006-2018 and 2021 NAICS codes. Issue: one company (EIN) can have multiple NAICS codes</t>
+  </si>
+  <si>
+    <t>2. Possible solution to 1.: combine RepUnit and EIN variables. Together, they make a company's location unique. However, a lot of observations have missing EINs too, which are either blank or coded as 0000000000</t>
+  </si>
+  <si>
+    <t>3. Considering UIN, EIN and rep_unit</t>
+  </si>
+  <si>
+    <t>1. Issue: MasterFile_2006Q1_2020Q4.dta was processed beforehand. When adding new data (2019,2020,2021), we see a difference of about 49%. Need code that created MasterFile_2006Q1_2020Q4.dta file so that succeeding years can also be cleaned.</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Time Period used</t>
+  </si>
+  <si>
+    <t>provided by</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>MasterFile_2006Q1_2020Q4.dta</t>
+  </si>
+  <si>
+    <t>2006Q1-2018Q4</t>
+  </si>
+  <si>
+    <t>Dr. Jones</t>
+  </si>
+  <si>
+    <t>C:\QCEW Data - Ohio\ES202</t>
+  </si>
+  <si>
+    <t>current_UCMA191.csv</t>
+  </si>
+  <si>
+    <t>2019Q1</t>
+  </si>
+  <si>
+    <t>Ohio JFS</t>
+  </si>
+  <si>
+    <t>current_UCMA192.csv</t>
+  </si>
+  <si>
+    <t>2019Q2</t>
+  </si>
+  <si>
+    <t>current_UCMA193.csv</t>
+  </si>
+  <si>
+    <t>2019Q3</t>
+  </si>
+  <si>
+    <t>current_UCMA194.csv</t>
+  </si>
+  <si>
+    <t>2019Q4</t>
+  </si>
+  <si>
+    <t>UC_2020_1.dta</t>
+  </si>
+  <si>
+    <t>2020Q1</t>
+  </si>
+  <si>
+    <t>UC_2020_2.dta</t>
+  </si>
+  <si>
+    <t>2020Q2</t>
+  </si>
+  <si>
+    <t>UC_2020_3.dta</t>
+  </si>
+  <si>
+    <t>2020Q3</t>
+  </si>
+  <si>
+    <t>UC_2020_4.dta</t>
+  </si>
+  <si>
+    <t>2020Q4</t>
+  </si>
+  <si>
+    <t>current_UCMA2021Q1.csv</t>
+  </si>
+  <si>
+    <t>2021Q1</t>
+  </si>
+  <si>
+    <t>C:\QCEW Data - Ohio\ES202\2021</t>
+  </si>
+  <si>
+    <t>current_UCMA2021Q2.csv</t>
+  </si>
+  <si>
+    <t>2021Q2</t>
+  </si>
+  <si>
+    <t>2. Sent Dr. Jones an email about this issue</t>
+  </si>
+  <si>
+    <t>1. Dr. Jones suggested to remove MEEI == 2 from all the new files before running. And it works! Old data () and new files match (or are sufficiently close) for year 2022. But the question is, why does it work? What is MEEI ==2?</t>
+  </si>
+  <si>
+    <t>2. I also need to ensure I remove individual "problematic" EINs from new files before appending</t>
+  </si>
+  <si>
+    <t>1. Cleaned sas code for creating master dataset and summary tables</t>
+  </si>
+  <si>
+    <t>2. Exported master df masterfile_2006q1_2021q2.sas7bdat</t>
+  </si>
+  <si>
+    <t>3. Data looks clean now for research/analysis</t>
   </si>
 </sst>
 </file>
@@ -289,7 +410,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -312,6 +433,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -324,7 +460,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1511,10 +1647,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5C4ECB-801C-4DCD-8982-324EF5EEDE57}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,7 +1724,7 @@
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="2">
         <v>44627</v>
       </c>
     </row>
@@ -1602,9 +1738,302 @@
         <v>72</v>
       </c>
     </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>44644</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>44657</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>44660</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39957068-B5E9-4A17-8906-002253F101F7}">
+  <dimension ref="D6:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="5">
+        <v>3</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="5">
+        <v>4</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="5">
+        <v>5</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="5">
+        <v>6</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="5">
+        <v>7</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="5">
+        <v>8</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="5">
+        <v>9</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D16" s="5">
+        <v>10</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D17" s="5">
+        <v>11</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1615,15 +2044,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010060C37653FBFDB34DA291AE7806E480FB" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f94e6187d2db220b108a9f3f0e9620ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9772973a-2681-4778-b4c7-fa785e6ae870" xmlns:ns4="bb53d160-e9b7-42e4-9639-85c2eeb2a294" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="319ae0e8b2240766e8bd2072e6b672dc" ns3:_="" ns4:_="">
     <xsd:import namespace="9772973a-2681-4778-b4c7-fa785e6ae870"/>
@@ -1852,32 +2272,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED66E2D0-0B6B-4411-AD46-1D3BA8F9882C}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="bb53d160-e9b7-42e4-9639-85c2eeb2a294"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9772973a-2681-4778-b4c7-fa785e6ae870"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9772973a-2681-4778-b4c7-fa785e6ae870"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{242C0C61-61DE-4A00-A79C-59E23BDFF550}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C0A05F-21D7-40FA-8438-69CD335DEFF2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1894,4 +2315,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{242C0C61-61DE-4A00-A79C-59E23BDFF550}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>